<commit_message>
correct misleading values in mapping schemes; revised area and cost assumptions for all occupancies; revised count assumptions for non-residential
</commit_message>
<xml_diff>
--- a/mapping_schemes/central/BDI_COM.xlsx
+++ b/mapping_schemes/central/BDI_COM.xlsx
@@ -4975,10 +4975,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>2600</v>
+        <v>130</v>
       </c>
       <c r="D2" t="n">
-        <v>545</v>
+        <v>218.0887622149837</v>
       </c>
       <c r="E2" t="n">
         <v>0.7</v>
@@ -4995,14 +4995,14 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Financial intermediation; insurance; real estate and business services</t>
+          <t>Professional and technical services</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>750</v>
+        <v>130</v>
       </c>
       <c r="D3" t="n">
-        <v>626</v>
+        <v>250.5019543973941</v>
       </c>
       <c r="E3" t="n">
         <v>0.25</v>
@@ -5019,14 +5019,14 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Community; social and personal services</t>
+          <t>All other services</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1000</v>
+        <v>130</v>
       </c>
       <c r="D4" t="n">
-        <v>565</v>
+        <v>226.0920195439739</v>
       </c>
       <c r="E4" t="n">
         <v>0.05</v>
@@ -5047,16 +5047,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>3100</v>
+        <v>260</v>
       </c>
       <c r="D5" t="n">
-        <v>545</v>
+        <v>218.0887622149837</v>
       </c>
       <c r="E5" t="n">
         <v>0.4</v>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
@@ -5067,20 +5067,20 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Financial intermediation; insurance; real estate and business services</t>
+          <t>Professional and technical services</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>950</v>
+        <v>260</v>
       </c>
       <c r="D6" t="n">
-        <v>626</v>
+        <v>250.5019543973941</v>
       </c>
       <c r="E6" t="n">
         <v>0.4</v>
       </c>
       <c r="F6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
@@ -5091,20 +5091,20 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Community; social and personal services</t>
+          <t>All other services</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1200</v>
+        <v>260</v>
       </c>
       <c r="D7" t="n">
-        <v>565</v>
+        <v>226.0920195439739</v>
       </c>
       <c r="E7" t="n">
         <v>0.2</v>
       </c>
       <c r="F7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
@@ -5119,16 +5119,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>3300</v>
+        <v>450</v>
       </c>
       <c r="D8" t="n">
-        <v>545</v>
+        <v>218.0887622149837</v>
       </c>
       <c r="E8" t="n">
         <v>0.1</v>
       </c>
       <c r="F8" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9">
@@ -5139,20 +5139,20 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Financial intermediation; insurance; real estate and business services</t>
+          <t>Professional and technical services</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1300</v>
+        <v>450</v>
       </c>
       <c r="D9" t="n">
-        <v>626</v>
+        <v>250.5019543973941</v>
       </c>
       <c r="E9" t="n">
         <v>0.8</v>
       </c>
       <c r="F9" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10">
@@ -5163,20 +5163,20 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Community; social and personal services</t>
+          <t>All other services</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>1500</v>
+        <v>450</v>
       </c>
       <c r="D10" t="n">
-        <v>565</v>
+        <v>226.0920195439739</v>
       </c>
       <c r="E10" t="n">
         <v>0.1</v>
       </c>
       <c r="F10" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11">
@@ -5191,16 +5191,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>5000</v>
+        <v>900</v>
       </c>
       <c r="D11" t="n">
-        <v>545</v>
+        <v>218.0887622149837</v>
       </c>
       <c r="E11" t="n">
         <v>0.05</v>
       </c>
       <c r="F11" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12">
@@ -5211,20 +5211,20 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Financial intermediation; insurance; real estate and business services</t>
+          <t>Professional and technical services</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>4500</v>
+        <v>900</v>
       </c>
       <c r="D12" t="n">
-        <v>626</v>
+        <v>250.5019543973941</v>
       </c>
       <c r="E12" t="n">
         <v>0.85</v>
       </c>
       <c r="F12" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13">
@@ -5235,20 +5235,20 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Community; social and personal services</t>
+          <t>All other services</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>4500</v>
+        <v>900</v>
       </c>
       <c r="D13" t="n">
-        <v>565</v>
+        <v>226.0920195439739</v>
       </c>
       <c r="E13" t="n">
         <v>0.1</v>
       </c>
       <c r="F13" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14">
@@ -5259,20 +5259,20 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Financial intermediation; insurance; real estate and business services</t>
+          <t>Professional and technical services</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>5100</v>
+        <v>1200</v>
       </c>
       <c r="D14" t="n">
-        <v>820</v>
+        <v>328.1335504885993</v>
       </c>
       <c r="E14" t="n">
         <v>0.05</v>
       </c>
       <c r="F14" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15">
@@ -5283,20 +5283,20 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Wholesale and retail trade</t>
+          <t>Professional and technical services</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>4500</v>
+        <v>1200</v>
       </c>
       <c r="D15" t="n">
-        <v>545</v>
+        <v>218.0887622149837</v>
       </c>
       <c r="E15" t="n">
         <v>0.85</v>
       </c>
       <c r="F15" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16">
@@ -5307,20 +5307,20 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Community; social and personal services</t>
+          <t>All other services</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>4000</v>
+        <v>1200</v>
       </c>
       <c r="D16" t="n">
-        <v>565</v>
+        <v>226.0920195439739</v>
       </c>
       <c r="E16" t="n">
         <v>0.1</v>
       </c>
       <c r="F16" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17">
@@ -5331,20 +5331,20 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Financial intermediation; insurance; real estate and business services</t>
+          <t>Professional and technical services</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>5400</v>
+        <v>3200</v>
       </c>
       <c r="D17" t="n">
-        <v>820</v>
+        <v>328.1335504885993</v>
       </c>
       <c r="E17" t="n">
         <v>0.85</v>
       </c>
       <c r="F17" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18">
@@ -5355,20 +5355,20 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Wholesale and retail trade</t>
+          <t>Professional and technical services</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>4500</v>
+        <v>3200</v>
       </c>
       <c r="D18" t="n">
-        <v>545</v>
+        <v>218.0887622149837</v>
       </c>
       <c r="E18" t="n">
         <v>0.05</v>
       </c>
       <c r="F18" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19">
@@ -5379,20 +5379,20 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Community; social and personal services</t>
+          <t>All other services</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>4000</v>
+        <v>3200</v>
       </c>
       <c r="D19" t="n">
-        <v>565</v>
+        <v>226.0920195439739</v>
       </c>
       <c r="E19" t="n">
         <v>0.1</v>
       </c>
       <c r="F19" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>